<commit_message>
Add climate control and pre-conditioning room documentation
- Fruiting room specifications (2.95x3.15x1.95m = 18.12m³)
- Environmental requirements for oyster and lion's mane
- Airflow calculations based on substrate load
- Pre-conditioning room sizing guidelines (~5-6m³)
- System layout diagram with air flow path
- Equipment specifications for Darwin climate
- AC sizing calculations (2.5kW minimum)
- Spore protection considerations
- Duct sizing (150mm insulated flex)

Also includes calculator fixes from earlier session.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/mushroom_calculator.xlsx
+++ b/mushroom_calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xavie\Documents\mushroom_farm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EC4784-BDD0-49B4-B08D-73803CCE7C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8668B877-C716-4855-ACE9-F0B320DB5F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50595" yWindow="900" windowWidth="25830" windowHeight="17415" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50595" yWindow="900" windowWidth="25830" windowHeight="17415" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Oyster" sheetId="1" r:id="rId1"/>
@@ -770,7 +770,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,7 +922,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="4">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>25</v>
@@ -936,7 +936,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="4">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>25</v>
@@ -950,7 +950,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="4">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>25</v>
@@ -964,7 +964,7 @@
         <v>31</v>
       </c>
       <c r="B17" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>25</v>
@@ -993,7 +993,7 @@
       </c>
       <c r="B19" s="5">
         <f>SUM(B14:B18)</f>
-        <v>6.3</v>
+        <v>9.5</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>25</v>
@@ -1016,7 +1016,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="4">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>38</v>
@@ -1130,15 +1130,15 @@
       </c>
       <c r="B33" s="9">
         <f>B5*B22</f>
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="C33" s="9">
         <f>B33*4.33</f>
-        <v>2165</v>
+        <v>3031</v>
       </c>
       <c r="D33" s="9">
         <f>B33*52</f>
-        <v>26000</v>
+        <v>36400</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1147,15 +1147,15 @@
       </c>
       <c r="B34" s="9">
         <f>B28*B19</f>
-        <v>100.8</v>
+        <v>152</v>
       </c>
       <c r="C34" s="9">
         <f>B34*4.33</f>
-        <v>436.464</v>
+        <v>658.16</v>
       </c>
       <c r="D34" s="9">
         <f>B34*52</f>
-        <v>5241.5999999999995</v>
+        <v>7904</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1164,15 +1164,15 @@
       </c>
       <c r="B35" s="5">
         <f>B33-B34</f>
-        <v>399.2</v>
+        <v>548</v>
       </c>
       <c r="C35" s="5">
         <f>C33-C34</f>
-        <v>1728.5360000000001</v>
+        <v>2372.84</v>
       </c>
       <c r="D35" s="5">
         <f>D33-D34</f>
-        <v>20758.400000000001</v>
+        <v>28496</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B36" s="10">
         <f>B35/B33</f>
-        <v>0.7984</v>
+        <v>0.78285714285714281</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="B39" s="11">
         <f>B19/B26</f>
-        <v>5.04</v>
+        <v>7.6</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>38</v>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B40" s="11">
         <f>B22-(B19/B26)</f>
-        <v>19.96</v>
+        <v>27.4</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>38</v>
@@ -1225,7 +1225,7 @@
       </c>
       <c r="B41" s="11">
         <f>(B22*B26)-B19</f>
-        <v>24.95</v>
+        <v>34.25</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>25</v>
@@ -1250,7 +1250,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,7 +1402,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>25</v>
@@ -1416,7 +1416,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>25</v>
@@ -1430,7 +1430,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="4">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>25</v>
@@ -1444,7 +1444,7 @@
         <v>31</v>
       </c>
       <c r="B17" s="4">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>25</v>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="B19" s="5">
         <f>SUM(B14:B18)</f>
-        <v>8.3000000000000007</v>
+        <v>10</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>25</v>
@@ -1496,7 +1496,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="4">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>38</v>
@@ -1610,15 +1610,15 @@
       </c>
       <c r="B33" s="9">
         <f>B5*B22</f>
-        <v>350</v>
+        <v>500</v>
       </c>
       <c r="C33" s="9">
         <f>B33*4.33</f>
-        <v>1515.5</v>
+        <v>2165</v>
       </c>
       <c r="D33" s="9">
         <f>B33*52</f>
-        <v>18200</v>
+        <v>26000</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1627,15 +1627,15 @@
       </c>
       <c r="B34" s="9">
         <f>B28*B19</f>
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="C34" s="9">
         <f>B34*4.33</f>
-        <v>359.39</v>
+        <v>433</v>
       </c>
       <c r="D34" s="9">
         <f>B34*52</f>
-        <v>4316</v>
+        <v>5200</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1644,15 +1644,15 @@
       </c>
       <c r="B35" s="5">
         <f>B33-B34</f>
-        <v>267</v>
+        <v>400</v>
       </c>
       <c r="C35" s="5">
         <f>C33-C34</f>
-        <v>1156.1100000000001</v>
+        <v>1732</v>
       </c>
       <c r="D35" s="5">
         <f>D33-D34</f>
-        <v>13884</v>
+        <v>20800</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="B36" s="10">
         <f>B35/B33</f>
-        <v>0.7628571428571429</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1678,7 +1678,7 @@
       </c>
       <c r="B39" s="11">
         <f>B19/B26</f>
-        <v>8.3000000000000007</v>
+        <v>10</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>38</v>
@@ -1693,7 +1693,7 @@
       </c>
       <c r="B40" s="11">
         <f>B22-(B19/B26)</f>
-        <v>26.7</v>
+        <v>40</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>38</v>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="B41" s="11">
         <f>(B22*B26)-B19</f>
-        <v>26.7</v>
+        <v>40</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>25</v>
@@ -1729,8 +1729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,11 +1831,11 @@
       </c>
       <c r="B8" s="13">
         <f>Oyster!B19</f>
-        <v>6.3</v>
+        <v>9.5</v>
       </c>
       <c r="C8" s="13">
         <f>'Lions Mane'!B19</f>
-        <v>8.3000000000000007</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1844,11 +1844,11 @@
       </c>
       <c r="B9" s="13">
         <f>Oyster!B22</f>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C9" s="13">
         <f>'Lions Mane'!B22</f>
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1879,15 +1879,15 @@
       </c>
       <c r="B13" s="9">
         <f>Oyster!B33</f>
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="C13" s="9">
         <f>'Lions Mane'!B33</f>
-        <v>350</v>
+        <v>500</v>
       </c>
       <c r="D13" s="11">
         <f>B13+C13</f>
-        <v>850</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1896,15 +1896,15 @@
       </c>
       <c r="B14" s="9">
         <f>Oyster!B34</f>
-        <v>100.8</v>
+        <v>152</v>
       </c>
       <c r="C14" s="9">
         <f>'Lions Mane'!B34</f>
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="D14" s="11">
         <f>B14+C14</f>
-        <v>183.8</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1913,15 +1913,15 @@
       </c>
       <c r="B15" s="9">
         <f>Oyster!B35</f>
-        <v>399.2</v>
+        <v>548</v>
       </c>
       <c r="C15" s="9">
         <f>'Lions Mane'!B35</f>
-        <v>267</v>
+        <v>400</v>
       </c>
       <c r="D15" s="5">
         <f>B15+C15</f>
-        <v>666.2</v>
+        <v>948</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1930,15 +1930,15 @@
       </c>
       <c r="B16" s="9">
         <f>Oyster!C35</f>
-        <v>1728.5360000000001</v>
+        <v>2372.84</v>
       </c>
       <c r="C16" s="9">
         <f>'Lions Mane'!C35</f>
-        <v>1156.1100000000001</v>
+        <v>1732</v>
       </c>
       <c r="D16" s="5">
         <f>B16+C16</f>
-        <v>2884.6460000000002</v>
+        <v>4104.84</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1947,15 +1947,15 @@
       </c>
       <c r="B17" s="9">
         <f>Oyster!D35</f>
-        <v>20758.400000000001</v>
+        <v>28496</v>
       </c>
       <c r="C17" s="9">
         <f>'Lions Mane'!D35</f>
-        <v>13884</v>
+        <v>20800</v>
       </c>
       <c r="D17" s="5">
         <f>B17+C17</f>
-        <v>34642.400000000001</v>
+        <v>49296</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2038,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2097,15 +2097,15 @@
       </c>
       <c r="D5" s="18">
         <f>(A5*Oyster!B22)-(B5*Oyster!B19)</f>
-        <v>99.8</v>
+        <v>137</v>
       </c>
       <c r="E5" s="18">
         <f t="shared" ref="E5:E12" si="0">D5*4.33</f>
-        <v>432.13400000000001</v>
+        <v>593.21</v>
       </c>
       <c r="F5" s="18">
         <f t="shared" ref="F5:F12" si="1">D5*52</f>
-        <v>5189.5999999999995</v>
+        <v>7124</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2122,15 +2122,15 @@
       </c>
       <c r="D6" s="18">
         <f>(A6*Oyster!B22)-(B6*Oyster!B19)</f>
-        <v>199.6</v>
+        <v>274</v>
       </c>
       <c r="E6" s="18">
         <f t="shared" si="0"/>
-        <v>864.26800000000003</v>
+        <v>1186.42</v>
       </c>
       <c r="F6" s="18">
         <f t="shared" si="1"/>
-        <v>10379.199999999999</v>
+        <v>14248</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2147,15 +2147,15 @@
       </c>
       <c r="D7" s="18">
         <f>(A7*Oyster!B22)-(B7*Oyster!B19)</f>
-        <v>299.39999999999998</v>
+        <v>411</v>
       </c>
       <c r="E7" s="18">
         <f t="shared" si="0"/>
-        <v>1296.4019999999998</v>
+        <v>1779.63</v>
       </c>
       <c r="F7" s="18">
         <f t="shared" si="1"/>
-        <v>15568.8</v>
+        <v>21372</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2172,15 +2172,15 @@
       </c>
       <c r="D8" s="18">
         <f>(A8*Oyster!B22)-(B8*Oyster!B19)</f>
-        <v>399.2</v>
+        <v>548</v>
       </c>
       <c r="E8" s="18">
         <f t="shared" si="0"/>
-        <v>1728.5360000000001</v>
+        <v>2372.84</v>
       </c>
       <c r="F8" s="18">
         <f t="shared" si="1"/>
-        <v>20758.399999999998</v>
+        <v>28496</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2197,15 +2197,15 @@
       </c>
       <c r="D9" s="18">
         <f>(A9*Oyster!B22)-(B9*Oyster!B19)</f>
-        <v>499</v>
+        <v>685</v>
       </c>
       <c r="E9" s="18">
         <f t="shared" si="0"/>
-        <v>2160.67</v>
+        <v>2966.05</v>
       </c>
       <c r="F9" s="18">
         <f t="shared" si="1"/>
-        <v>25948</v>
+        <v>35620</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2222,15 +2222,15 @@
       </c>
       <c r="D10" s="18">
         <f>(A10*Oyster!B22)-(B10*Oyster!B19)</f>
-        <v>598.79999999999995</v>
+        <v>822</v>
       </c>
       <c r="E10" s="18">
         <f t="shared" si="0"/>
-        <v>2592.8039999999996</v>
+        <v>3559.26</v>
       </c>
       <c r="F10" s="18">
         <f t="shared" si="1"/>
-        <v>31137.599999999999</v>
+        <v>42744</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2247,15 +2247,15 @@
       </c>
       <c r="D11" s="18">
         <f>(A11*Oyster!B22)-(B11*Oyster!B19)</f>
-        <v>798.4</v>
+        <v>1096</v>
       </c>
       <c r="E11" s="18">
         <f t="shared" si="0"/>
-        <v>3457.0720000000001</v>
+        <v>4745.68</v>
       </c>
       <c r="F11" s="18">
         <f t="shared" si="1"/>
-        <v>41516.799999999996</v>
+        <v>56992</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2272,15 +2272,15 @@
       </c>
       <c r="D12" s="18">
         <f>(A12*Oyster!B22)-(B12*Oyster!B19)</f>
-        <v>998</v>
+        <v>1370</v>
       </c>
       <c r="E12" s="18">
         <f t="shared" si="0"/>
-        <v>4321.34</v>
+        <v>5932.1</v>
       </c>
       <c r="F12" s="18">
         <f t="shared" si="1"/>
-        <v>51896</v>
+        <v>71240</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2322,15 +2322,15 @@
       </c>
       <c r="D17" s="18">
         <f>(A17*'Lions Mane'!B22)-(B17*'Lions Mane'!B19)</f>
-        <v>80.099999999999994</v>
+        <v>120</v>
       </c>
       <c r="E17" s="18">
         <f t="shared" ref="E17:E23" si="2">D17*4.33</f>
-        <v>346.83299999999997</v>
+        <v>519.6</v>
       </c>
       <c r="F17" s="18">
         <f t="shared" ref="F17:F23" si="3">D17*52</f>
-        <v>4165.2</v>
+        <v>6240</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2347,15 +2347,15 @@
       </c>
       <c r="D18" s="18">
         <f>(A18*'Lions Mane'!B22)-(B18*'Lions Mane'!B19)</f>
-        <v>133.5</v>
+        <v>200</v>
       </c>
       <c r="E18" s="18">
         <f t="shared" si="2"/>
-        <v>578.05500000000006</v>
+        <v>866</v>
       </c>
       <c r="F18" s="18">
         <f t="shared" si="3"/>
-        <v>6942</v>
+        <v>10400</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2372,15 +2372,15 @@
       </c>
       <c r="D19" s="18">
         <f>(A19*'Lions Mane'!B22)-(B19*'Lions Mane'!B19)</f>
-        <v>213.6</v>
+        <v>320</v>
       </c>
       <c r="E19" s="18">
         <f t="shared" si="2"/>
-        <v>924.88800000000003</v>
+        <v>1385.6</v>
       </c>
       <c r="F19" s="18">
         <f t="shared" si="3"/>
-        <v>11107.199999999999</v>
+        <v>16640</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2397,15 +2397,15 @@
       </c>
       <c r="D20" s="18">
         <f>(A20*'Lions Mane'!B22)-(B20*'Lions Mane'!B19)</f>
-        <v>267</v>
+        <v>400</v>
       </c>
       <c r="E20" s="18">
         <f t="shared" si="2"/>
-        <v>1156.1100000000001</v>
+        <v>1732</v>
       </c>
       <c r="F20" s="18">
         <f t="shared" si="3"/>
-        <v>13884</v>
+        <v>20800</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2422,15 +2422,15 @@
       </c>
       <c r="D21" s="18">
         <f>(A21*'Lions Mane'!B22)-(B21*'Lions Mane'!B19)</f>
-        <v>320.39999999999998</v>
+        <v>480</v>
       </c>
       <c r="E21" s="18">
         <f t="shared" si="2"/>
-        <v>1387.3319999999999</v>
+        <v>2078.4</v>
       </c>
       <c r="F21" s="18">
         <f t="shared" si="3"/>
-        <v>16660.8</v>
+        <v>24960</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2447,15 +2447,15 @@
       </c>
       <c r="D22" s="18">
         <f>(A22*'Lions Mane'!B22)-(B22*'Lions Mane'!B19)</f>
-        <v>400.5</v>
+        <v>600</v>
       </c>
       <c r="E22" s="18">
         <f t="shared" si="2"/>
-        <v>1734.165</v>
+        <v>2598</v>
       </c>
       <c r="F22" s="18">
         <f t="shared" si="3"/>
-        <v>20826</v>
+        <v>31200</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2472,15 +2472,15 @@
       </c>
       <c r="D23" s="18">
         <f>(A23*'Lions Mane'!B22)-(B23*'Lions Mane'!B19)</f>
-        <v>534</v>
+        <v>800</v>
       </c>
       <c r="E23" s="18">
         <f t="shared" si="2"/>
-        <v>2312.2200000000003</v>
+        <v>3464</v>
       </c>
       <c r="F23" s="18">
         <f t="shared" si="3"/>
-        <v>27768</v>
+        <v>41600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>